<commit_message>
added all the data
</commit_message>
<xml_diff>
--- a/cro/Grand_slam_table_norm.xlsx
+++ b/cro/Grand_slam_table_norm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Documents\GitHub\Grand-Slam-database\cro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C1BA70-BE18-4FDA-AEF2-0D4AEF0AFB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B0EEA8-7B14-4A70-BD40-E5A9578FA979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B936E176-7309-4377-81B0-28528B1442FB}"/>
   </bookViews>
@@ -641,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BDFD43C-0EC4-4D8E-9742-8E5A2867B58E}">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -914,12 +914,8 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E17" s="5">
-        <v>83</v>
-      </c>
-      <c r="F17" s="5">
-        <v>5</v>
-      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">

</xml_diff>